<commit_message>
minor changes to the sentiment analysis.
</commit_message>
<xml_diff>
--- a/src/data/sentiment_results/sentiment_results_subset_bert.xlsx
+++ b/src/data/sentiment_results/sentiment_results_subset_bert.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="270">
   <si>
     <t>Row_Number</t>
   </si>
@@ -538,286 +538,289 @@
     <t>negative</t>
   </si>
   <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5916969180107117}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5693313479423523}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5895366072654724}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6036034822463989}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6080217361450195}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.588270366191864}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5854630470275879}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5944741368293762}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5938578248023987}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.562719464302063}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5757389664649963}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.566905677318573}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5971829891204834}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5956318974494934}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5861929059028625}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.5091389417648315}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6106927394866943}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5862908363342285}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5709123015403748}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.589354395866394}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5670754909515381}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.584679901599884}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5691462755203247}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.567473828792572}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5866484642028809}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.607661247253418}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5871456861495972}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6097240447998047}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5856868028640747}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6035250425338745}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6204073429107666}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6088345050811768}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5873022079467773}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5880128741264343}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5763501524925232}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5701358318328857}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.589832067489624}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6046820878982544}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5684308409690857}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5902097821235657}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5865317583084106}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6097988486289978}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6036753058433533}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.578697681427002}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5764983296394348}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6012349724769592}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5918165445327759}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5981040000915527}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6010522246360779}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5554327368736267}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6054760813713074}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6005452275276184}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5921173095703125}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6002692580223083}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6082077622413635}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5825232863426208}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5871391892433167}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5876449942588806}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5949013233184814}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5620637536048889}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5855088233947754}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5908483266830444}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5811583995819092}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.5759962797164917}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5628423690795898}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.579218864440918}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5711125135421753}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6056495904922485}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6038333773612976}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5997419357299805}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5922433137893677}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5794576406478882}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5929903984069824}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.595542848110199}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.569464921951294}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6002998352050781}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5800025463104248}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5926781892776489}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5940556526184082}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6044471263885498}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5938553214073181}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5970156192779541}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6083683371543884}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5875859260559082}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5955032706260681}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6048761606216431}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5765437483787537}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5974059104919434}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5902712345123291}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.6093481183052063}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5882217884063721}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5709911584854126}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.602209746837616}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_1', 'score': 0.5990084409713745}</t>
+    <t>{'label': 'LABEL_0', 'score': 0.6165294051170349}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6152240633964539}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6276030540466309}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6287968158721924}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6265703439712524}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6092011332511902}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6154984831809998}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6121871471405029}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6297902464866638}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6118900179862976}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6316757798194885}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6154239177703857}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6156269311904907}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.623571515083313}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6084762215614319}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.5984631776809692}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6161437034606934}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6115897297859192}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6084784269332886}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6260745525360107}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6434668302536011}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.626284658908844}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.612806499004364}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6143962740898132}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6199201345443726}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6308311820030212}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6215488910675049}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.644977867603302}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6224562525749207}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6275407075881958}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6146340370178223}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6022341847419739}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6090781092643738}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6110119819641113}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.648396909236908}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6297367811203003}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.62285977602005}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6285818219184875}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6175370216369629}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6186134815216064}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6211050152778625}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.612415611743927}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6200401782989502}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6257834434509277}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6227863430976868}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6207936406135559}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6283147931098938}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6177467703819275}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.618755578994751}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6097444295883179}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6146154999732971}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6213558912277222}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6223445534706116}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6208321452140808}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.649174153804779}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.59809410572052}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6069620847702026}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6127477884292603}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6205687522888184}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6281725168228149}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6178492307662964}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6152944564819336}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6149681210517883}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.622868001461029}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6356972455978394}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6169376373291016}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6011926531791687}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6514390707015991}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6188256740570068}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6082078218460083}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6253708600997925}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6273909211158752}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6172049045562744}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6198626756668091}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6217631101608276}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6265097856521606}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6118432879447937}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6141948103904724}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6261197924613953}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6199622750282288}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6402068138122559}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.612963080406189}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6144188046455383}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.613923966884613}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6049232482910156}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6211430430412292}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6153357028961182}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.5993615388870239}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6199654936790466}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6265184879302979}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6110716462135315}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6054821610450745}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6227136254310608}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6235061287879944}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6221509575843811}</t>
   </si>
   <si>
     <t>Negative</t>
@@ -1239,7 +1242,7 @@
         <v>174</v>
       </c>
       <c r="I2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1268,7 +1271,7 @@
         <v>175</v>
       </c>
       <c r="I3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1297,7 +1300,7 @@
         <v>176</v>
       </c>
       <c r="I4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1326,7 +1329,7 @@
         <v>177</v>
       </c>
       <c r="I5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1355,7 +1358,7 @@
         <v>178</v>
       </c>
       <c r="I6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1384,7 +1387,7 @@
         <v>179</v>
       </c>
       <c r="I7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1413,7 +1416,7 @@
         <v>180</v>
       </c>
       <c r="I8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1442,7 +1445,7 @@
         <v>181</v>
       </c>
       <c r="I9" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1471,7 +1474,7 @@
         <v>182</v>
       </c>
       <c r="I10" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1500,7 +1503,7 @@
         <v>183</v>
       </c>
       <c r="I11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1529,7 +1532,7 @@
         <v>184</v>
       </c>
       <c r="I12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1558,7 +1561,7 @@
         <v>185</v>
       </c>
       <c r="I13" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1587,7 +1590,7 @@
         <v>186</v>
       </c>
       <c r="I14" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1616,7 +1619,7 @@
         <v>187</v>
       </c>
       <c r="I15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1645,7 +1648,7 @@
         <v>188</v>
       </c>
       <c r="I16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1674,7 +1677,7 @@
         <v>189</v>
       </c>
       <c r="I17" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1703,7 +1706,7 @@
         <v>190</v>
       </c>
       <c r="I18" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1732,7 +1735,7 @@
         <v>191</v>
       </c>
       <c r="I19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1761,7 +1764,7 @@
         <v>192</v>
       </c>
       <c r="I20" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1790,7 +1793,7 @@
         <v>193</v>
       </c>
       <c r="I21" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1819,7 +1822,7 @@
         <v>194</v>
       </c>
       <c r="I22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1848,7 +1851,7 @@
         <v>195</v>
       </c>
       <c r="I23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1877,7 +1880,7 @@
         <v>196</v>
       </c>
       <c r="I24" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1906,7 +1909,7 @@
         <v>197</v>
       </c>
       <c r="I25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1935,7 +1938,7 @@
         <v>198</v>
       </c>
       <c r="I26" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1964,7 +1967,7 @@
         <v>198</v>
       </c>
       <c r="I27" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1993,7 +1996,7 @@
         <v>199</v>
       </c>
       <c r="I28" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2022,7 +2025,7 @@
         <v>200</v>
       </c>
       <c r="I29" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2051,7 +2054,7 @@
         <v>201</v>
       </c>
       <c r="I30" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2080,7 +2083,7 @@
         <v>202</v>
       </c>
       <c r="I31" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2109,7 +2112,7 @@
         <v>203</v>
       </c>
       <c r="I32" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2138,7 +2141,7 @@
         <v>203</v>
       </c>
       <c r="I33" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2167,7 +2170,7 @@
         <v>203</v>
       </c>
       <c r="I34" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2196,7 +2199,7 @@
         <v>204</v>
       </c>
       <c r="I35" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2225,7 +2228,7 @@
         <v>205</v>
       </c>
       <c r="I36" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2254,7 +2257,7 @@
         <v>206</v>
       </c>
       <c r="I37" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2283,7 +2286,7 @@
         <v>207</v>
       </c>
       <c r="I38" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2312,7 +2315,7 @@
         <v>208</v>
       </c>
       <c r="I39" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2341,7 +2344,7 @@
         <v>209</v>
       </c>
       <c r="I40" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2370,7 +2373,7 @@
         <v>210</v>
       </c>
       <c r="I41" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2399,7 +2402,7 @@
         <v>211</v>
       </c>
       <c r="I42" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2428,7 +2431,7 @@
         <v>212</v>
       </c>
       <c r="I43" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2457,7 +2460,7 @@
         <v>213</v>
       </c>
       <c r="I44" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2486,7 +2489,7 @@
         <v>214</v>
       </c>
       <c r="I45" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2515,7 +2518,7 @@
         <v>215</v>
       </c>
       <c r="I46" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2544,7 +2547,7 @@
         <v>216</v>
       </c>
       <c r="I47" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2573,7 +2576,7 @@
         <v>217</v>
       </c>
       <c r="I48" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2602,7 +2605,7 @@
         <v>218</v>
       </c>
       <c r="I49" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2631,7 +2634,7 @@
         <v>219</v>
       </c>
       <c r="I50" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2660,7 +2663,7 @@
         <v>220</v>
       </c>
       <c r="I51" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2689,7 +2692,7 @@
         <v>221</v>
       </c>
       <c r="I52" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2718,7 +2721,7 @@
         <v>222</v>
       </c>
       <c r="I53" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2747,7 +2750,7 @@
         <v>223</v>
       </c>
       <c r="I54" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2776,7 +2779,7 @@
         <v>224</v>
       </c>
       <c r="I55" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2805,7 +2808,7 @@
         <v>225</v>
       </c>
       <c r="I56" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2834,7 +2837,7 @@
         <v>226</v>
       </c>
       <c r="I57" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2863,7 +2866,7 @@
         <v>227</v>
       </c>
       <c r="I58" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2892,7 +2895,7 @@
         <v>228</v>
       </c>
       <c r="I59" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2921,7 +2924,7 @@
         <v>229</v>
       </c>
       <c r="I60" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2950,7 +2953,7 @@
         <v>230</v>
       </c>
       <c r="I61" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2979,7 +2982,7 @@
         <v>227</v>
       </c>
       <c r="I62" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -3008,7 +3011,7 @@
         <v>231</v>
       </c>
       <c r="I63" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3037,7 +3040,7 @@
         <v>232</v>
       </c>
       <c r="I64" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3066,7 +3069,7 @@
         <v>233</v>
       </c>
       <c r="I65" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3095,7 +3098,7 @@
         <v>234</v>
       </c>
       <c r="I66" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -3124,7 +3127,7 @@
         <v>235</v>
       </c>
       <c r="I67" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3153,7 +3156,7 @@
         <v>236</v>
       </c>
       <c r="I68" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3182,7 +3185,7 @@
         <v>237</v>
       </c>
       <c r="I69" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3211,7 +3214,7 @@
         <v>238</v>
       </c>
       <c r="I70" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -3240,7 +3243,7 @@
         <v>239</v>
       </c>
       <c r="I71" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3266,10 +3269,10 @@
         <v>172</v>
       </c>
       <c r="H72" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="I72" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3295,10 +3298,10 @@
         <v>173</v>
       </c>
       <c r="H73" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I73" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3324,10 +3327,10 @@
         <v>173</v>
       </c>
       <c r="H74" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I74" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3353,10 +3356,10 @@
         <v>171</v>
       </c>
       <c r="H75" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I75" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3382,10 +3385,10 @@
         <v>173</v>
       </c>
       <c r="H76" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I76" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3411,10 +3414,10 @@
         <v>172</v>
       </c>
       <c r="H77" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="I77" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3440,10 +3443,10 @@
         <v>173</v>
       </c>
       <c r="H78" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I78" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3469,10 +3472,10 @@
         <v>172</v>
       </c>
       <c r="H79" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I79" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3498,10 +3501,10 @@
         <v>171</v>
       </c>
       <c r="H80" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I80" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3527,10 +3530,10 @@
         <v>171</v>
       </c>
       <c r="H81" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I81" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3556,10 +3559,10 @@
         <v>173</v>
       </c>
       <c r="H82" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I82" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3585,10 +3588,10 @@
         <v>173</v>
       </c>
       <c r="H83" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I83" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3614,10 +3617,10 @@
         <v>172</v>
       </c>
       <c r="H84" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I84" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3643,10 +3646,10 @@
         <v>173</v>
       </c>
       <c r="H85" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I85" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3672,10 +3675,10 @@
         <v>171</v>
       </c>
       <c r="H86" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I86" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3701,10 +3704,10 @@
         <v>173</v>
       </c>
       <c r="H87" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I87" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3730,10 +3733,10 @@
         <v>173</v>
       </c>
       <c r="H88" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I88" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3759,10 +3762,10 @@
         <v>173</v>
       </c>
       <c r="H89" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I89" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3788,10 +3791,10 @@
         <v>171</v>
       </c>
       <c r="H90" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I90" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3817,10 +3820,10 @@
         <v>171</v>
       </c>
       <c r="H91" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I91" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3846,10 +3849,10 @@
         <v>172</v>
       </c>
       <c r="H92" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I92" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3875,10 +3878,10 @@
         <v>173</v>
       </c>
       <c r="H93" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I93" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3904,10 +3907,10 @@
         <v>171</v>
       </c>
       <c r="H94" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I94" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3933,10 +3936,10 @@
         <v>173</v>
       </c>
       <c r="H95" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I95" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3962,10 +3965,10 @@
         <v>172</v>
       </c>
       <c r="H96" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I96" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3991,10 +3994,10 @@
         <v>171</v>
       </c>
       <c r="H97" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I97" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -4020,10 +4023,10 @@
         <v>171</v>
       </c>
       <c r="H98" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I98" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -4049,10 +4052,10 @@
         <v>173</v>
       </c>
       <c r="H99" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I99" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -4078,10 +4081,10 @@
         <v>171</v>
       </c>
       <c r="H100" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I100" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -4107,10 +4110,10 @@
         <v>171</v>
       </c>
       <c r="H101" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I101" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added further visuals to sentiment_analysis.ipynb
</commit_message>
<xml_diff>
--- a/src/data/sentiment_results/sentiment_results_subset_bert.xlsx
+++ b/src/data/sentiment_results/sentiment_results_subset_bert.xlsx
@@ -538,289 +538,289 @@
     <t>negative</t>
   </si>
   <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6165294051170349}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6152240633964539}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6276030540466309}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6287968158721924}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6265703439712524}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6092011332511902}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6154984831809998}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6121871471405029}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6297902464866638}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6118900179862976}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6316757798194885}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6154239177703857}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6156269311904907}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.623571515083313}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6084762215614319}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.5984631776809692}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6161437034606934}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6115897297859192}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6084784269332886}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6260745525360107}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6434668302536011}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.626284658908844}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.612806499004364}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6143962740898132}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6199201345443726}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6308311820030212}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6215488910675049}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.644977867603302}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6224562525749207}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6275407075881958}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6146340370178223}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6022341847419739}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6090781092643738}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6110119819641113}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.648396909236908}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6297367811203003}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.62285977602005}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6285818219184875}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6175370216369629}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6186134815216064}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6211050152778625}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.612415611743927}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6200401782989502}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6257834434509277}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6227863430976868}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6207936406135559}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6283147931098938}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6177467703819275}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.618755578994751}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6097444295883179}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6146154999732971}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6213558912277222}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6223445534706116}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6208321452140808}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.649174153804779}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.59809410572052}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6069620847702026}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6127477884292603}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6205687522888184}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6281725168228149}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6178492307662964}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6152944564819336}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6149681210517883}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.622868001461029}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6356972455978394}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6169376373291016}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6011926531791687}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6514390707015991}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6188256740570068}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6082078218460083}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6253708600997925}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6273909211158752}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6172049045562744}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6198626756668091}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6217631101608276}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6265097856521606}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6118432879447937}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6141948103904724}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6261197924613953}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6199622750282288}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6402068138122559}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.612963080406189}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6144188046455383}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.613923966884613}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6049232482910156}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6211430430412292}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6153357028961182}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.5993615388870239}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6199654936790466}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6265184879302979}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6110716462135315}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6054821610450745}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6227136254310608}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6235061287879944}</t>
-  </si>
-  <si>
-    <t>{'label': 'LABEL_0', 'score': 0.6221509575843811}</t>
+    <t>{'label': 'LABEL_0', 'score': 0.7060643434524536}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7031141519546509}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7124890685081482}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6995008587837219}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7029309272766113}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7012220025062561}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7027474641799927}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6979803442955017}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7009510397911072}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7117259502410889}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7162072658538818}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7009451985359192}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7081892490386963}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7122577428817749}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.694705069065094}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6902344822883606}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7087001204490662}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7044041156768799}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7215670347213745}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7173374891281128}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6990979909896851}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7108794450759888}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6965128183364868}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7174103856086731}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.714772641658783}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6991731524467468}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7042048573493958}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7437578439712524}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7018510103225708}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.712437629699707}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7006770372390747}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6990013718605042}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7057111263275146}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6992059946060181}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6891406178474426}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6955220699310303}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7196774482727051}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7043949365615845}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6948150396347046}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6972740292549133}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6998518705368042}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6952220797538757}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7081985473632812}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7076496481895447}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7043262720108032}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7235633134841919}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7047570943832397}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.693343997001648}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.711338222026825}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7013468742370605}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6828898787498474}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6985781788825989}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7072131037712097}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7100904583930969}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7125943303108215}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7129694223403931}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6952589154243469}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7134063243865967}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7165772318840027}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7070124745368958}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7149694561958313}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7006003260612488}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6897069811820984}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7066183090209961}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6868455410003662}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7175314426422119}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7129970192909241}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7049190998077393}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6992518305778503}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6826577186584473}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7148903012275696}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7103974223136902}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6986395120620728}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7201886773109436}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7090784311294556}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7135809659957886}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6985413432121277}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7058203816413879}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7120464444160461}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.71199631690979}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7189050316810608}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6927416324615479}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.713079571723938}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6928613781929016}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7136166095733643}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7095724940299988}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7074331641197205}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6991096138954163}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7003313899040222}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7140833139419556}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7046642899513245}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6973547339439392}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7223910093307495}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.6902124881744385}</t>
+  </si>
+  <si>
+    <t>{'label': 'LABEL_0', 'score': 0.7040569186210632}</t>
   </si>
   <si>
     <t>Negative</t>

</xml_diff>